<commit_message>
use sorghum to determine the deleterious alleles.
</commit_message>
<xml_diff>
--- a/data/snpeff_results.xlsx
+++ b/data/snpeff_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangjl/Documents/Github/GERP-diallel/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangjl/Documents/Github/myprojects/GERP-diallel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t xml:space="preserve">Type </t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>UTR</t>
+  </si>
+  <si>
+    <t>synonymous_variant</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,6 +672,9 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
       <c r="B22">
         <f>SUM(B9,B14:B16)</f>
         <v>65376</v>

</xml_diff>